<commit_message>
Labb2 first atempt at 1c
</commit_message>
<xml_diff>
--- a/Labb2/data/betyg_o_prov_riksnivå.xlsx
+++ b/Labb2/data/betyg_o_prov_riksnivå.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Tabell 1A"/>
@@ -1382,7 +1382,7 @@
   </sheetPr>
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2465,7 +2465,7 @@
   </sheetPr>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Weird bugg error on 1.c debugged and fixed
</commit_message>
<xml_diff>
--- a/Labb2/data/betyg_o_prov_riksnivå.xlsx
+++ b/Labb2/data/betyg_o_prov_riksnivå.xlsx
@@ -500,6 +500,12 @@
       <sz val="12"/>
       <color rgb="FF0000ff"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -546,12 +552,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -799,61 +799,61 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -880,52 +880,52 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -949,19 +949,19 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -976,13 +976,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="12" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1030,31 +1030,31 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">

</xml_diff>